<commit_message>
pdate regex for md5 value checking
</commit_message>
<xml_diff>
--- a/reads/reads_schema_main_v0.1.xlsx
+++ b/reads/reads_schema_main_v0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zef22hak/development/COPO_refactoring/COPO-production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD21C1F-4552-4049-BA3A-E2C9A0D3379E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025A0D79-9E0C-814A-82F6-C95205E53645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7BD8D0E6-E1F4-E04F-9790-31602B31B6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="1256">
   <si>
     <t>component_name</t>
   </si>
@@ -3533,12 +3533,6 @@
     <t>sequencing_annotation_file_type</t>
   </si>
   <si>
-    <t>sequencing_annotation_file_name</t>
-  </si>
-  <si>
-    <t>assembly_file_name</t>
-  </si>
-  <si>
     <t>Sequencing Annotation ID</t>
   </si>
   <si>
@@ -3834,6 +3828,24 @@
   </si>
   <si>
     <t>LIBPREP</t>
+  </si>
+  <si>
+    <t>sequencing_annotation_file_checksum</t>
+  </si>
+  <si>
+    <t>File Checksum</t>
+  </si>
+  <si>
+    <t>assembly_file_checksum</t>
+  </si>
+  <si>
+    <t>^[0-9a-f]{32}$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it must be a hex number with  32 digits </t>
+  </si>
+  <si>
+    <t>it must be a  hex number with 32 digits</t>
   </si>
 </sst>
 </file>
@@ -5133,12 +5145,12 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S91"/>
+  <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A23" sqref="A23"/>
-      <selection pane="topRight" activeCell="G33" sqref="G33"/>
+      <selection pane="topRight" activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5183,7 +5195,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>6</v>
@@ -5210,16 +5222,16 @@
         <v>13</v>
       </c>
       <c r="P1" s="18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>1171</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>1172</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="S1" s="57" t="s">
         <v>1173</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>1174</v>
-      </c>
-      <c r="S1" s="57" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -6643,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>190</v>
@@ -6837,7 +6849,7 @@
         <v>217</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="F36" s="1" t="b">
         <v>0</v>
@@ -6878,7 +6890,7 @@
         <v>219</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>219</v>
@@ -6922,7 +6934,7 @@
         <v>221</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>221</v>
@@ -6966,7 +6978,7 @@
         <v>223</v>
       </c>
       <c r="D39" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>223</v>
@@ -7007,16 +7019,16 @@
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="F40" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -7159,7 +7171,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>228</v>
@@ -7299,7 +7311,7 @@
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>15</v>
@@ -7352,7 +7364,7 @@
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>15</v>
@@ -7367,13 +7379,13 @@
         <v>1</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>267</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="K47" s="3" t="s">
         <v>20</v>
@@ -7403,7 +7415,7 @@
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>15</v>
@@ -7454,7 +7466,7 @@
     </row>
     <row r="49" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>15</v>
@@ -7505,7 +7517,7 @@
     </row>
     <row r="50" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>15</v>
@@ -7549,7 +7561,7 @@
     </row>
     <row r="51" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>15</v>
@@ -7593,7 +7605,7 @@
     </row>
     <row r="52" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>15</v>
@@ -7613,8 +7625,12 @@
       <c r="J52" s="44" t="s">
         <v>1104</v>
       </c>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
+      <c r="K52" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>1254</v>
+      </c>
       <c r="M52" s="3" t="s">
         <v>22</v>
       </c>
@@ -7637,7 +7653,7 @@
     </row>
     <row r="53" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>15</v>
@@ -7657,8 +7673,12 @@
       <c r="J53" s="44" t="s">
         <v>1104</v>
       </c>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
+      <c r="K53" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>1255</v>
+      </c>
       <c r="M53" s="3" t="s">
         <v>22</v>
       </c>
@@ -7681,13 +7701,13 @@
     </row>
     <row r="54" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>283</v>
@@ -7793,7 +7813,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>1129</v>
@@ -8071,7 +8091,7 @@
     </row>
     <row r="63" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="51" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B63" s="51" t="s">
         <v>15</v>
@@ -8124,28 +8144,28 @@
     </row>
     <row r="64" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="44" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="F64" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="J64" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>20</v>
@@ -8172,7 +8192,7 @@
     </row>
     <row r="65" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>15</v>
@@ -8222,28 +8242,28 @@
     </row>
     <row r="66" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="44" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="F66" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>1143</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="K66" s="3" t="s">
         <v>20</v>
@@ -8331,22 +8351,22 @@
         <v>15</v>
       </c>
       <c r="C68" s="44" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="F68" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="J68" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="K68" s="3" t="s">
         <v>20</v>
@@ -8606,22 +8626,22 @@
         <v>15</v>
       </c>
       <c r="C74" s="44" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="D74" s="44" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="F74" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="J74" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>20</v>
@@ -8736,7 +8756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1114</v>
       </c>
@@ -8744,7 +8764,7 @@
         <v>15</v>
       </c>
       <c r="C77" s="44" t="s">
-        <v>1152</v>
+        <v>1114</v>
       </c>
       <c r="D77" t="s">
         <v>282</v>
@@ -8774,87 +8794,85 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="47" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B78" s="47" t="s">
+    <row r="78" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E78" s="47"/>
-      <c r="F78" s="51" t="b">
+      <c r="C78" s="44" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F78" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G78" s="51"/>
-      <c r="H78" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="I78" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="J78" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="K78" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="L78" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="M78" t="s">
+      <c r="I78" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="J78" s="44" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="M78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N78" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P78" s="45" t="s">
+      <c r="O78" s="3"/>
+      <c r="P78" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="Q78" s="69" t="s">
+      <c r="Q78" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="R78" s="69" t="s">
+      <c r="R78" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="S78" s="46" t="s">
+      <c r="S78" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B79" s="3" t="s">
+    <row r="79" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="47" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B79" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="44" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D79" t="s">
-        <v>1153</v>
-      </c>
-      <c r="F79" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>1246</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>1159</v>
-      </c>
-      <c r="J79" t="s">
-        <v>1161</v>
-      </c>
-      <c r="K79" s="3" t="s">
+      <c r="C79" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D79" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="47"/>
+      <c r="F79" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" s="51"/>
+      <c r="H79" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J79" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K79" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L79" s="3" t="s">
+      <c r="L79" s="47" t="s">
         <v>21</v>
       </c>
       <c r="M79" t="s">
@@ -8878,28 +8896,28 @@
     </row>
     <row r="80" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C80" s="44" t="s">
-        <v>155</v>
+        <v>1149</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>1151</v>
       </c>
       <c r="F80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>153</v>
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>1244</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>1135</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>158</v>
+        <v>1157</v>
+      </c>
+      <c r="J80" t="s">
+        <v>1159</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>20</v>
@@ -8928,22 +8946,31 @@
     </row>
     <row r="81" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C81" s="44" t="s">
-        <v>1165</v>
+        <v>155</v>
       </c>
       <c r="D81" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="F81" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="H81" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="I81" s="3" t="s">
-        <v>1167</v>
+        <v>1135</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>21</v>
@@ -8967,24 +8994,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="44" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="D82" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F82" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>1168</v>
+        <v>1165</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="M82" t="s">
         <v>22</v>
@@ -8992,51 +9022,37 @@
       <c r="N82" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P82" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q82" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="R82" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="S82" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="47" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B83" s="47" t="s">
+      <c r="P82" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q82" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="R82" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="S82" s="46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D83" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="47"/>
-      <c r="F83" s="51" t="b">
+      <c r="C83" s="44" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D83" t="s">
+        <v>39</v>
+      </c>
+      <c r="F83" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G83" s="51"/>
-      <c r="H83" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="I83" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="J83" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="K83" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="L83" s="47" t="s">
-        <v>21</v>
+      <c r="I83" s="3" t="s">
+        <v>1166</v>
       </c>
       <c r="M83" t="s">
         <v>22</v>
@@ -9044,48 +9060,50 @@
       <c r="N83" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P83" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q83" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="R83" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="S83" s="46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B84" s="3" t="s">
+      <c r="P83" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q83" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="R83" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="S83" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="47" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B84" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="44" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D84" t="s">
-        <v>1228</v>
-      </c>
-      <c r="F84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>1247</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="J84" t="s">
-        <v>1239</v>
-      </c>
-      <c r="K84" s="3" t="s">
+      <c r="C84" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" s="47"/>
+      <c r="F84" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" s="51"/>
+      <c r="H84" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J84" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K84" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L84" s="3" t="s">
+      <c r="L84" s="47" t="s">
         <v>21</v>
       </c>
       <c r="M84" t="s">
@@ -9109,28 +9127,28 @@
     </row>
     <row r="85" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="44" t="s">
-        <v>1149</v>
+        <v>1225</v>
       </c>
       <c r="D85" t="s">
-        <v>1153</v>
+        <v>1226</v>
       </c>
       <c r="F85" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>1154</v>
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>1245</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>1159</v>
+        <v>1232</v>
       </c>
       <c r="J85" t="s">
-        <v>1161</v>
+        <v>1237</v>
       </c>
       <c r="K85" s="3" t="s">
         <v>20</v>
@@ -9157,27 +9175,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C86" s="44" t="s">
-        <v>1196</v>
-      </c>
-      <c r="D86" s="44" t="s">
-        <v>1214</v>
+        <v>1149</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1151</v>
       </c>
       <c r="F86" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>1190</v>
+        <v>1152</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>1143</v>
+        <v>1157</v>
+      </c>
+      <c r="J86" t="s">
+        <v>1159</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="M86" t="s">
         <v>22</v>
@@ -9198,38 +9225,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="47" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B87" s="47" t="s">
+    <row r="87" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D87" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" s="48"/>
-      <c r="F87" s="51" t="b">
+      <c r="C87" s="44" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D87" s="44" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F87" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G87" s="51"/>
-      <c r="H87" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="J87" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="K87" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="L87" s="47" t="s">
-        <v>21</v>
+      <c r="H87" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>1143</v>
       </c>
       <c r="M87" t="s">
         <v>22</v>
@@ -9250,35 +9266,37 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B88" s="3" t="s">
+    <row r="88" spans="1:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="47" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B88" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="44" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D88" t="s">
-        <v>1230</v>
-      </c>
-      <c r="F88" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>1248</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>1235</v>
-      </c>
-      <c r="J88" t="s">
-        <v>1240</v>
-      </c>
-      <c r="K88" s="3" t="s">
+      <c r="C88" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" s="48"/>
+      <c r="F88" s="51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" s="51"/>
+      <c r="H88" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="J88" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K88" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L88" s="3" t="s">
+      <c r="L88" s="47" t="s">
         <v>21</v>
       </c>
       <c r="M88" t="s">
@@ -9302,28 +9320,28 @@
     </row>
     <row r="89" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C89" s="44" t="s">
-        <v>1149</v>
+        <v>1227</v>
       </c>
       <c r="D89" t="s">
-        <v>1153</v>
+        <v>1228</v>
       </c>
       <c r="F89" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>1154</v>
+        <v>1</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>1246</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>1159</v>
+        <v>1233</v>
       </c>
       <c r="J89" t="s">
-        <v>1161</v>
+        <v>1238</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>20</v>
@@ -9352,28 +9370,40 @@
     </row>
     <row r="90" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C90" s="44" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="D90" t="s">
-        <v>283</v>
+        <v>1151</v>
       </c>
       <c r="F90" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="I90" t="s">
-        <v>1160</v>
+      <c r="H90" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="J90" t="s">
+        <v>1159</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="M90" t="s">
         <v>22</v>
       </c>
-      <c r="N90" t="s">
-        <v>59</v>
+      <c r="N90" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="P90" s="45" t="s">
         <v>24</v>
@@ -9390,28 +9420,28 @@
     </row>
     <row r="91" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C91" s="44" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D91" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F91" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="M91" t="s">
         <v>22</v>
       </c>
-      <c r="N91" s="3" t="s">
-        <v>253</v>
+      <c r="N91" t="s">
+        <v>59</v>
       </c>
       <c r="P91" s="45" t="s">
         <v>24</v>
@@ -9423,13 +9453,99 @@
         <v>24</v>
       </c>
       <c r="S91" s="46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D92" t="s">
+        <v>282</v>
+      </c>
+      <c r="F92" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>1161</v>
+      </c>
+      <c r="M92" t="s">
+        <v>22</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="P92" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q92" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="R92" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="S92" s="46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="44" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="J93" s="44" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="L93" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="M93" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O93" s="3"/>
+      <c r="P93" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q93" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="R93" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="S93" s="25" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S54" xr:uid="{545CA0C1-0282-3A43-9C60-512DE414A571}"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S26:S30 P2:R91" xr:uid="{D3C8CE10-E7EB-B24A-855C-B8189CB5A06C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S26:S30 P2:R93" xr:uid="{D3C8CE10-E7EB-B24A-855C-B8189CB5A06C}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="O3" r:id="rId1" xr:uid="{4D6B5FE8-0E6D-E84F-B3F9-D5B11E30DF9B}"/>
@@ -9706,7 +9822,7 @@
         <v>231</v>
       </c>
       <c r="BE1" s="42" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="BF1" s="13" t="s">
         <v>1110</v>
@@ -9870,7 +9986,7 @@
         <v>343</v>
       </c>
       <c r="AX2" s="34" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="AY2" s="16" t="s">
         <v>344</v>
@@ -9889,7 +10005,7 @@
       </c>
       <c r="BD2" s="36"/>
       <c r="BE2" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="BF2" t="s">
         <v>1122</v>
@@ -9901,7 +10017,7 @@
         <v>1137</v>
       </c>
       <c r="BI2" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="3" spans="1:61" ht="20" x14ac:dyDescent="0.25">
@@ -10049,7 +10165,7 @@
         <v>381</v>
       </c>
       <c r="AX3" s="16" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="AY3" s="16" t="s">
         <v>382</v>
@@ -10080,7 +10196,7 @@
         <v>1138</v>
       </c>
       <c r="BI3" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="4" spans="1:61" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -10212,7 +10328,7 @@
         <v>415</v>
       </c>
       <c r="AX4" s="16" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="AY4" s="16" t="s">
         <v>416</v>
@@ -10231,7 +10347,7 @@
       </c>
       <c r="BD4" s="36"/>
       <c r="BE4" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="BG4" t="s">
         <v>1119</v>
@@ -10240,7 +10356,7 @@
         <v>1139</v>
       </c>
       <c r="BI4" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="5" spans="1:61" ht="20" x14ac:dyDescent="0.25">
@@ -10362,7 +10478,7 @@
         <v>447</v>
       </c>
       <c r="AX5" s="16" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="AY5" s="16" t="s">
         <v>448</v>
@@ -10381,13 +10497,13 @@
       </c>
       <c r="BD5" s="36"/>
       <c r="BE5" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="BH5" t="s">
         <v>1140</v>
       </c>
       <c r="BI5" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="6" spans="1:61" ht="20" x14ac:dyDescent="0.25">
@@ -10495,7 +10611,7 @@
         <v>474</v>
       </c>
       <c r="AX6" s="16" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="AY6" s="16" t="s">
         <v>475</v>
@@ -10608,7 +10724,7 @@
         <v>496</v>
       </c>
       <c r="AX7" s="16" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="AY7" s="16" t="s">
         <v>497</v>
@@ -10712,7 +10828,7 @@
         <v>513</v>
       </c>
       <c r="AX8" s="16" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="AY8" s="16" t="s">
         <v>514</v>
@@ -10808,7 +10924,7 @@
         <v>528</v>
       </c>
       <c r="AX9" s="16" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="AY9" s="16" t="s">
         <v>529</v>
@@ -10890,7 +11006,7 @@
         <v>538</v>
       </c>
       <c r="AX10" s="16" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="AY10" s="16" t="s">
         <v>539</v>
@@ -10972,7 +11088,7 @@
         <v>548</v>
       </c>
       <c r="AX11" s="16" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="AY11" s="16" t="s">
         <v>549</v>
@@ -11048,7 +11164,7 @@
         <v>556</v>
       </c>
       <c r="AX12" s="16" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="AY12" s="16" t="s">
         <v>557</v>
@@ -11122,7 +11238,7 @@
         <v>563</v>
       </c>
       <c r="AX13" s="16" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="AY13" s="16" t="s">
         <v>564</v>
@@ -11196,7 +11312,7 @@
         <v>570</v>
       </c>
       <c r="AX14" s="16" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="AY14" s="16" t="s">
         <v>571</v>
@@ -11268,7 +11384,7 @@
         <v>576</v>
       </c>
       <c r="AX15" s="16" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="AY15" s="16" t="s">
         <v>577</v>
@@ -11340,7 +11456,7 @@
         <v>582</v>
       </c>
       <c r="AX16" s="16" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="AY16" s="16" t="s">
         <v>583</v>
@@ -11412,7 +11528,7 @@
         <v>588</v>
       </c>
       <c r="AX17" s="16" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="AY17" s="16" t="s">
         <v>589</v>
@@ -28851,13 +28967,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="B2" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="C2" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="D2" t="s">
         <v>1067</v>
@@ -28868,13 +28984,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B3" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C3" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -28885,13 +29001,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="B4" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="C4" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="D4" t="s">
         <v>185</v>
@@ -28902,13 +29018,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="B5" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C5" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="D5" t="s">
         <v>90</v>
@@ -29003,10 +29119,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C7" t="s">
         <v>1077</v>
@@ -29028,15 +29144,15 @@
         <v>1115</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -29044,34 +29160,34 @@
         <v>1114</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>1107</v>
       </c>
       <c r="C12" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
   </sheetData>
@@ -29356,12 +29472,12 @@
         <v>256</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>260</v>

</xml_diff>